<commit_message>
Add Visual Studio files and remove dependency on ntoh*/hton* functions
</commit_message>
<xml_diff>
--- a/Tori.xlsx
+++ b/Tori.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin.Spinar\Documents\Visual Studio 2015\Projects\tori_c\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alipha\Documents\Visual Studio 2013\Projects\tori_c\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20970" windowHeight="4410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19395" windowHeight="1440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="59">
   <si>
     <t>To Entry</t>
   </si>
@@ -173,9 +173,6 @@
     <t>Routes</t>
   </si>
   <si>
-    <t>134 per</t>
-  </si>
-  <si>
     <t>For packet retransmission</t>
   </si>
   <si>
@@ -183,6 +180,27 @@
   </si>
   <si>
     <t>Move this into connection packet, but that means we need a changing nonce (note that this is based upon userId, not connectionId)</t>
+  </si>
+  <si>
+    <t>Connect Data</t>
+  </si>
+  <si>
+    <t>AddressType</t>
+  </si>
+  <si>
+    <t>DestAddress</t>
+  </si>
+  <si>
+    <t>Up to 256</t>
+  </si>
+  <si>
+    <t>DestPort</t>
+  </si>
+  <si>
+    <t>TotalRouteCount</t>
+  </si>
+  <si>
+    <t>102 per</t>
   </si>
 </sst>
 </file>
@@ -198,7 +216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +259,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -254,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -289,6 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,25 +935,25 @@
         <v>2</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K11" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N11" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q11" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="S11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -951,22 +976,22 @@
         <v>8</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="K12" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="N12" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="Q12" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -989,22 +1014,22 @@
         <v>2</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="N13" s="2">
+        <v>2</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1027,22 +1052,22 @@
         <v>36</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N14" s="2">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1065,22 +1090,22 @@
         <v>1</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K15" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N15" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q15" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1103,23 +1128,22 @@
         <v>2</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L16" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="K16" s="2">
+        <v>2</v>
+      </c>
       <c r="M16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="N16" s="2">
+        <v>2</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -1142,23 +1166,23 @@
         <v>18</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -1180,23 +1204,23 @@
       <c r="H18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K18" s="4">
+      <c r="J18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N18" s="2">
+        <v>17</v>
+      </c>
+      <c r="N18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q18" s="2">
+        <v>17</v>
+      </c>
+      <c r="Q18" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1219,12 +1243,25 @@
       <c r="H19">
         <v>16</v>
       </c>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
+      <c r="J19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="4">
+        <v>16</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="M19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N19" s="2">
+        <v>16</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
@@ -1263,9 +1300,7 @@
       <c r="H21" s="8">
         <v>41</v>
       </c>
-      <c r="J21" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -1284,26 +1319,31 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="J22" s="4" t="s">
-        <v>38</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="K22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
       <c r="S22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="K23" t="s">
-        <v>39</v>
-      </c>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
+      <c r="J23" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>43</v>
       </c>
       <c r="K24" t="s">
-        <v>40</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1312,11 +1352,8 @@
       <c r="D25">
         <v>4</v>
       </c>
-      <c r="J25" t="s">
-        <v>42</v>
-      </c>
-      <c r="K25">
-        <v>4</v>
+      <c r="K25" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -1326,14 +1363,11 @@
       <c r="D26">
         <v>8</v>
       </c>
-      <c r="J26" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K26" s="4">
-        <v>32</v>
-      </c>
-      <c r="M26" t="s">
-        <v>52</v>
+      <c r="J26" t="s">
+        <v>42</v>
+      </c>
+      <c r="K26">
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -1343,71 +1377,114 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="J27" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K27" s="4">
-        <v>8</v>
+      <c r="J27" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="M27" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
-      </c>
-      <c r="J28" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="4">
+        <v>8</v>
+      </c>
+      <c r="M28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="J29" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="K28" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="J29" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="K29" s="9">
-        <v>1</v>
+      <c r="K29" s="4">
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="J30" s="7" t="s">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K30" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="J31" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="K30" s="7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="J31" s="11" t="s">
+      <c r="K31" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="K31" s="7">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="J32" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="K32" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J33" s="8" t="s">
+      <c r="K32" s="7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K33" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="J34" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K33" s="8">
-        <v>16</v>
-      </c>
-      <c r="M33" t="s">
+      <c r="K34" s="8">
+        <v>16</v>
+      </c>
+      <c r="M34" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>